<commit_message>
Exportar Odenes Modificacion -Estable-
</commit_message>
<xml_diff>
--- a/SOP_IAA/Plantillas/Factor_Reajuste.xlsx
+++ b/SOP_IAA/Plantillas/Factor_Reajuste.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Descripcion</t>
   </si>
@@ -42,7 +42,16 @@
     <t>Item</t>
   </si>
   <si>
-    <t xml:space="preserve">FACTORES  DE REAJUSTES </t>
+    <t>FACTORES  DE REAJUSTE</t>
+  </si>
+  <si>
+    <t>Lugar</t>
+  </si>
+  <si>
+    <t>Zona</t>
+  </si>
+  <si>
+    <t>Contratación</t>
   </si>
 </sst>
 </file>
@@ -56,7 +65,7 @@
     <numFmt numFmtId="166" formatCode="&quot;¢&quot;_(* #\ \ ###\ \ ###.00_);[Red]&quot;¢&quot;_(* #\ ###\ ###.00_);_(&quot;¢&quot;* &quot;0.00&quot;_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="&quot;Autorizado &quot;0&quot; dc&quot;"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -116,6 +125,16 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -206,7 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -238,11 +257,16 @@
     <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
@@ -301,6 +325,7 @@
       <sheetName val="Programa"/>
       <sheetName val="Vinculos Descriptiva"/>
       <sheetName val="Control Boletas"/>
+      <sheetName val="FactorReajuste"/>
       <sheetName val="OM"/>
       <sheetName val="OS"/>
       <sheetName val="Fact "/>
@@ -440,49 +465,44 @@
       <sheetName val="Hoja3"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32">
-        <row r="10">
-          <cell r="C10" t="str">
-            <v>LP N°2009-000003-CV</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36">
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37">
         <row r="19">
           <cell r="A19" t="str">
             <v>ITEM</v>
@@ -2178,142 +2198,142 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
-      <sheetData sheetId="53" refreshError="1"/>
-      <sheetData sheetId="54" refreshError="1"/>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
-      <sheetData sheetId="57" refreshError="1"/>
-      <sheetData sheetId="58" refreshError="1"/>
-      <sheetData sheetId="59" refreshError="1"/>
-      <sheetData sheetId="60" refreshError="1"/>
-      <sheetData sheetId="61" refreshError="1"/>
-      <sheetData sheetId="62" refreshError="1"/>
-      <sheetData sheetId="63" refreshError="1"/>
-      <sheetData sheetId="64" refreshError="1"/>
-      <sheetData sheetId="65" refreshError="1"/>
-      <sheetData sheetId="66" refreshError="1"/>
-      <sheetData sheetId="67" refreshError="1"/>
-      <sheetData sheetId="68" refreshError="1"/>
-      <sheetData sheetId="69" refreshError="1"/>
-      <sheetData sheetId="70" refreshError="1"/>
-      <sheetData sheetId="71" refreshError="1"/>
-      <sheetData sheetId="72" refreshError="1"/>
-      <sheetData sheetId="73" refreshError="1"/>
-      <sheetData sheetId="74" refreshError="1"/>
-      <sheetData sheetId="75" refreshError="1"/>
-      <sheetData sheetId="76" refreshError="1"/>
-      <sheetData sheetId="77" refreshError="1"/>
-      <sheetData sheetId="78" refreshError="1"/>
-      <sheetData sheetId="79" refreshError="1"/>
-      <sheetData sheetId="80" refreshError="1"/>
-      <sheetData sheetId="81" refreshError="1"/>
-      <sheetData sheetId="82" refreshError="1"/>
-      <sheetData sheetId="83" refreshError="1"/>
-      <sheetData sheetId="84" refreshError="1"/>
-      <sheetData sheetId="85" refreshError="1"/>
-      <sheetData sheetId="86" refreshError="1"/>
-      <sheetData sheetId="87" refreshError="1"/>
-      <sheetData sheetId="88" refreshError="1"/>
-      <sheetData sheetId="89" refreshError="1"/>
-      <sheetData sheetId="90" refreshError="1"/>
-      <sheetData sheetId="91" refreshError="1"/>
-      <sheetData sheetId="92" refreshError="1"/>
-      <sheetData sheetId="93" refreshError="1"/>
-      <sheetData sheetId="94" refreshError="1"/>
-      <sheetData sheetId="95" refreshError="1"/>
-      <sheetData sheetId="96" refreshError="1"/>
-      <sheetData sheetId="97" refreshError="1"/>
-      <sheetData sheetId="98" refreshError="1"/>
-      <sheetData sheetId="99" refreshError="1"/>
-      <sheetData sheetId="100" refreshError="1"/>
-      <sheetData sheetId="101" refreshError="1"/>
-      <sheetData sheetId="102" refreshError="1"/>
-      <sheetData sheetId="103" refreshError="1"/>
-      <sheetData sheetId="104" refreshError="1"/>
-      <sheetData sheetId="105" refreshError="1"/>
-      <sheetData sheetId="106" refreshError="1"/>
-      <sheetData sheetId="107" refreshError="1"/>
-      <sheetData sheetId="108" refreshError="1"/>
-      <sheetData sheetId="109" refreshError="1"/>
-      <sheetData sheetId="110" refreshError="1"/>
-      <sheetData sheetId="111" refreshError="1"/>
-      <sheetData sheetId="112" refreshError="1"/>
-      <sheetData sheetId="113" refreshError="1"/>
-      <sheetData sheetId="114" refreshError="1"/>
-      <sheetData sheetId="115" refreshError="1"/>
-      <sheetData sheetId="116" refreshError="1"/>
-      <sheetData sheetId="117" refreshError="1"/>
-      <sheetData sheetId="118" refreshError="1"/>
-      <sheetData sheetId="119" refreshError="1"/>
-      <sheetData sheetId="120" refreshError="1"/>
-      <sheetData sheetId="121" refreshError="1"/>
-      <sheetData sheetId="122" refreshError="1"/>
-      <sheetData sheetId="123" refreshError="1"/>
-      <sheetData sheetId="124" refreshError="1"/>
-      <sheetData sheetId="125" refreshError="1"/>
-      <sheetData sheetId="126" refreshError="1"/>
-      <sheetData sheetId="127" refreshError="1"/>
-      <sheetData sheetId="128" refreshError="1"/>
-      <sheetData sheetId="129" refreshError="1"/>
-      <sheetData sheetId="130" refreshError="1"/>
-      <sheetData sheetId="131" refreshError="1"/>
-      <sheetData sheetId="132" refreshError="1"/>
-      <sheetData sheetId="133" refreshError="1"/>
-      <sheetData sheetId="134" refreshError="1"/>
-      <sheetData sheetId="135" refreshError="1"/>
-      <sheetData sheetId="136" refreshError="1"/>
-      <sheetData sheetId="137" refreshError="1"/>
-      <sheetData sheetId="138" refreshError="1"/>
-      <sheetData sheetId="139" refreshError="1"/>
-      <sheetData sheetId="140" refreshError="1"/>
-      <sheetData sheetId="141" refreshError="1"/>
-      <sheetData sheetId="142" refreshError="1"/>
-      <sheetData sheetId="143" refreshError="1"/>
-      <sheetData sheetId="144" refreshError="1"/>
-      <sheetData sheetId="145" refreshError="1"/>
-      <sheetData sheetId="146" refreshError="1"/>
-      <sheetData sheetId="147" refreshError="1"/>
-      <sheetData sheetId="148" refreshError="1"/>
-      <sheetData sheetId="149" refreshError="1"/>
-      <sheetData sheetId="150" refreshError="1"/>
-      <sheetData sheetId="151" refreshError="1"/>
-      <sheetData sheetId="152" refreshError="1"/>
-      <sheetData sheetId="153" refreshError="1"/>
-      <sheetData sheetId="154" refreshError="1"/>
-      <sheetData sheetId="155" refreshError="1"/>
-      <sheetData sheetId="156" refreshError="1"/>
-      <sheetData sheetId="157" refreshError="1"/>
-      <sheetData sheetId="158" refreshError="1"/>
-      <sheetData sheetId="159" refreshError="1"/>
-      <sheetData sheetId="160" refreshError="1"/>
-      <sheetData sheetId="161" refreshError="1"/>
-      <sheetData sheetId="162" refreshError="1"/>
-      <sheetData sheetId="163" refreshError="1"/>
-      <sheetData sheetId="164" refreshError="1"/>
-      <sheetData sheetId="165" refreshError="1"/>
-      <sheetData sheetId="166" refreshError="1"/>
-      <sheetData sheetId="167" refreshError="1"/>
-      <sheetData sheetId="168" refreshError="1"/>
-      <sheetData sheetId="169" refreshError="1"/>
-      <sheetData sheetId="170" refreshError="1"/>
-      <sheetData sheetId="171" refreshError="1"/>
-      <sheetData sheetId="172" refreshError="1"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
+      <sheetData sheetId="53"/>
+      <sheetData sheetId="54"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
+      <sheetData sheetId="58"/>
+      <sheetData sheetId="59"/>
+      <sheetData sheetId="60"/>
+      <sheetData sheetId="61"/>
+      <sheetData sheetId="62"/>
+      <sheetData sheetId="63"/>
+      <sheetData sheetId="64"/>
+      <sheetData sheetId="65"/>
+      <sheetData sheetId="66"/>
+      <sheetData sheetId="67"/>
+      <sheetData sheetId="68"/>
+      <sheetData sheetId="69"/>
+      <sheetData sheetId="70"/>
+      <sheetData sheetId="71"/>
+      <sheetData sheetId="72"/>
+      <sheetData sheetId="73"/>
+      <sheetData sheetId="74"/>
+      <sheetData sheetId="75"/>
+      <sheetData sheetId="76"/>
+      <sheetData sheetId="77"/>
+      <sheetData sheetId="78"/>
+      <sheetData sheetId="79"/>
+      <sheetData sheetId="80"/>
+      <sheetData sheetId="81"/>
+      <sheetData sheetId="82"/>
+      <sheetData sheetId="83"/>
+      <sheetData sheetId="84"/>
+      <sheetData sheetId="85"/>
+      <sheetData sheetId="86"/>
+      <sheetData sheetId="87"/>
+      <sheetData sheetId="88"/>
+      <sheetData sheetId="89"/>
+      <sheetData sheetId="90"/>
+      <sheetData sheetId="91"/>
+      <sheetData sheetId="92"/>
+      <sheetData sheetId="93"/>
+      <sheetData sheetId="94"/>
+      <sheetData sheetId="95"/>
+      <sheetData sheetId="96"/>
+      <sheetData sheetId="97"/>
+      <sheetData sheetId="98"/>
+      <sheetData sheetId="99"/>
+      <sheetData sheetId="100"/>
+      <sheetData sheetId="101"/>
+      <sheetData sheetId="102"/>
+      <sheetData sheetId="103"/>
+      <sheetData sheetId="104"/>
+      <sheetData sheetId="105"/>
+      <sheetData sheetId="106"/>
+      <sheetData sheetId="107"/>
+      <sheetData sheetId="108"/>
+      <sheetData sheetId="109"/>
+      <sheetData sheetId="110"/>
+      <sheetData sheetId="111"/>
+      <sheetData sheetId="112"/>
+      <sheetData sheetId="113"/>
+      <sheetData sheetId="114"/>
+      <sheetData sheetId="115"/>
+      <sheetData sheetId="116"/>
+      <sheetData sheetId="117"/>
+      <sheetData sheetId="118"/>
+      <sheetData sheetId="119"/>
+      <sheetData sheetId="120"/>
+      <sheetData sheetId="121"/>
+      <sheetData sheetId="122"/>
+      <sheetData sheetId="123"/>
+      <sheetData sheetId="124"/>
+      <sheetData sheetId="125"/>
+      <sheetData sheetId="126"/>
+      <sheetData sheetId="127"/>
+      <sheetData sheetId="128"/>
+      <sheetData sheetId="129"/>
+      <sheetData sheetId="130"/>
+      <sheetData sheetId="131"/>
+      <sheetData sheetId="132"/>
+      <sheetData sheetId="133"/>
+      <sheetData sheetId="134"/>
+      <sheetData sheetId="135"/>
+      <sheetData sheetId="136"/>
+      <sheetData sheetId="137"/>
+      <sheetData sheetId="138"/>
+      <sheetData sheetId="139"/>
+      <sheetData sheetId="140"/>
+      <sheetData sheetId="141"/>
+      <sheetData sheetId="142"/>
+      <sheetData sheetId="143"/>
+      <sheetData sheetId="144"/>
+      <sheetData sheetId="145"/>
+      <sheetData sheetId="146"/>
+      <sheetData sheetId="147"/>
+      <sheetData sheetId="148"/>
+      <sheetData sheetId="149"/>
+      <sheetData sheetId="150"/>
+      <sheetData sheetId="151"/>
+      <sheetData sheetId="152"/>
+      <sheetData sheetId="153"/>
+      <sheetData sheetId="154"/>
+      <sheetData sheetId="155"/>
+      <sheetData sheetId="156"/>
+      <sheetData sheetId="157"/>
+      <sheetData sheetId="158"/>
+      <sheetData sheetId="159"/>
+      <sheetData sheetId="160"/>
+      <sheetData sheetId="161"/>
+      <sheetData sheetId="162"/>
+      <sheetData sheetId="163"/>
+      <sheetData sheetId="164"/>
+      <sheetData sheetId="165"/>
+      <sheetData sheetId="166"/>
+      <sheetData sheetId="167"/>
+      <sheetData sheetId="168"/>
+      <sheetData sheetId="169"/>
+      <sheetData sheetId="170"/>
+      <sheetData sheetId="171"/>
+      <sheetData sheetId="172"/>
+      <sheetData sheetId="173"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2670,48 +2690,54 @@
   <dimension ref="B1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="82" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+    <row r="1" spans="2:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="B1" s="16"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="16"/>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+    <row r="2" spans="2:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="B2" s="16"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="16"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="17"/>
+    <row r="3" spans="2:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>5</v>
+      </c>
       <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="17"/>
+    <row r="4" spans="2:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>3</v>
+      </c>
       <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="17"/>
+    <row r="5" spans="2:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
+        <v>4</v>
+      </c>
       <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="D5" s="16"/>
     </row>
-    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="16"/>
-      <c r="C6" s="15"/>
+    <row r="6" spans="2:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="B6" s="15"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="9"/>
     </row>
     <row r="7" spans="2:4" ht="44.25" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="14"/>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="12"/>
@@ -2742,5 +2768,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>